<commit_message>
Update .gitignore and save file path in app.py
</commit_message>
<xml_diff>
--- a/dados_transportadoras_vtex_completos.xlsx
+++ b/dados_transportadoras_vtex_completos.xlsx
@@ -1180,7 +1180,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>American Express, Visa, Mastercard, Boleto Bancário, Hipercard, Elo, Vale, Pix, Diners, WH Google Pay</t>
+          <t>American Express, Visa, Mastercard, Boleto Bancário, Hipercard, Elo, Vale, Pix, WH Google Pay, Diners</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1234,7 +1234,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>American Express, Visa, Mastercard, Boleto Bancário, Hipercard, Elo, Vale, Pix, Diners, WH Google Pay</t>
+          <t>American Express, Visa, Mastercard, Boleto Bancário, Hipercard, Elo, Vale, Pix, WH Google Pay, Diners</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>American Express, Visa, Mastercard, Boleto Bancário, Hipercard, Elo, Vale, Pix, Diners, WH Google Pay</t>
+          <t>American Express, Visa, Mastercard, Boleto Bancário, Hipercard, Elo, Vale, Pix, WH Google Pay, Diners</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>American Express, Visa, Mastercard, Boleto Bancário, Hipercard, Elo, Vale, Pix, Diners, WH Google Pay</t>
+          <t>American Express, Visa, Mastercard, Boleto Bancário, Hipercard, Elo, Vale, Pix, WH Google Pay, Diners</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1396,7 +1396,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>American Express, Visa, Mastercard, Boleto Bancário, Hipercard, Elo, Vale, Pix, Diners, WH Google Pay</t>
+          <t>American Express, Visa, Mastercard, Boleto Bancário, Hipercard, Elo, Vale, Pix, WH Google Pay, Diners</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">

</xml_diff>